<commit_message>
dev of account syste
</commit_message>
<xml_diff>
--- a/gameData/shared/Errors.xlsx
+++ b/gameData/shared/Errors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1720" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="5520" yWindow="840" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="errors" sheetId="24" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="247">
   <si>
     <t>STR_key</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -865,6 +865,70 @@
   </si>
   <si>
     <t>订单验证失败</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩家已加入了联盟</t>
+  </si>
+  <si>
+    <t>playerAlreadyJoinAlliance</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>联盟名称已经存在</t>
+  </si>
+  <si>
+    <t>allianceNameExist</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>联盟标签已经存在</t>
+  </si>
+  <si>
+    <t>allianceTagExist</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>allianceOperationRightsIllegal</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>联盟操作权限不足</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>联盟荣耀值不足</t>
+  </si>
+  <si>
+    <t>allianceHonourNotEnough</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>联盟没有此玩家</t>
+  </si>
+  <si>
+    <t>allianceDoNotHasThisMember</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>联盟正在战争准备期或战争期,不能将玩家踢出联盟</t>
+  </si>
+  <si>
+    <t>allianceInFightStatusCanNotKickMemberOff</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>不能将职级高于或等于自己的玩家踢出联盟</t>
+  </si>
+  <si>
+    <t>canNotKickAllianceMemberOffForTitleIsUpperThanMe</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>别逗了,你是不盟主好么</t>
+  </si>
+  <si>
+    <t>youAreNotTheAllianceArchon</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1003,7 +1067,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1046">
+  <cellStyleXfs count="1118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -2054,6 +2118,78 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2067,7 +2203,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1046">
+  <cellStyles count="1118">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -2593,6 +2729,42 @@
     <cellStyle name="超链接" xfId="1040" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="1042" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="1044" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1046" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1048" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1050" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1052" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1054" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1056" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1058" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1060" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1062" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1064" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1066" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1068" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1070" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1072" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1074" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1076" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1078" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1080" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1082" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1084" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1086" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1088" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1090" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1092" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1094" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1096" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1098" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1100" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1102" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1104" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1106" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1108" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1110" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1112" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1114" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1116" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -3111,6 +3283,42 @@
     <cellStyle name="访问过的超链接" xfId="1041" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="1043" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="1045" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1047" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1049" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1051" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1053" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1055" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1057" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1059" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1061" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1063" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1065" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1067" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1069" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1071" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1073" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1075" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1077" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1079" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1081" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1083" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1085" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1087" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1089" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1091" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1093" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1095" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1097" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1099" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1101" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1103" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1105" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1107" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1109" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1111" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1113" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1115" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1117" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -3560,10 +3768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4826,6 +5034,105 @@
         <v>228</v>
       </c>
     </row>
+    <row r="115" spans="1:3" ht="20" customHeight="1">
+      <c r="A115" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B115" s="1">
+        <v>614</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="20" customHeight="1">
+      <c r="A116" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B116" s="1">
+        <v>615</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="20" customHeight="1">
+      <c r="A117" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B117" s="1">
+        <v>616</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="20" customHeight="1">
+      <c r="A118" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B118" s="1">
+        <v>617</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="20" customHeight="1">
+      <c r="A119" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B119" s="1">
+        <v>618</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="20" customHeight="1">
+      <c r="A120" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B120" s="1">
+        <v>619</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="20" customHeight="1">
+      <c r="A121" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B121" s="1">
+        <v>620</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="20" customHeight="1">
+      <c r="A122" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B122" s="1">
+        <v>621</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="20" customHeight="1">
+      <c r="A123" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B123" s="1">
+        <v>622</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
dev of account systen
</commit_message>
<xml_diff>
--- a/gameData/shared/Errors.xlsx
+++ b/gameData/shared/Errors.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="353">
   <si>
     <t>STR_key</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -1297,7 +1297,23 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>playerAlreadyBindGCAccountId</t>
+    <t>此GameCenter账号已有玩家数据</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>此GameCenter账号下无玩家数据</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>playerAlreadyBindGCAId</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>theGCIdAlreadyHasDatas</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>theGCAccountDoNotHasData</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1436,7 +1452,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1568">
+  <cellStyleXfs count="1594">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -3009,6 +3025,32 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3022,7 +3064,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1568">
+  <cellStyles count="1594">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -3809,6 +3851,19 @@
     <cellStyle name="超链接" xfId="1562" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="1564" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="1566" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1568" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1570" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1572" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1574" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1576" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1578" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1580" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1582" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1584" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1586" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1588" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1590" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1592" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -4588,6 +4643,19 @@
     <cellStyle name="访问过的超链接" xfId="1563" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="1565" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="1567" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1569" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1571" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1573" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1575" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1577" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1579" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1581" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1583" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1585" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1587" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1589" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1591" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1593" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -5037,10 +5105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="D154" sqref="D154"/>
+      <selection activeCell="A177" sqref="A177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6954,13 +7022,35 @@
     </row>
     <row r="174" spans="1:3" ht="20" customHeight="1">
       <c r="A174" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B174" s="1">
         <v>673</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>347</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="20" customHeight="1">
+      <c r="A175" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B175" s="1">
+        <v>674</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="20" customHeight="1">
+      <c r="A176" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B176" s="1">
+        <v>675</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev of gm tools
</commit_message>
<xml_diff>
--- a/gameData/shared/Errors.xlsx
+++ b/gameData/shared/Errors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="5720" yWindow="300" windowWidth="28360" windowHeight="19660" tabRatio="883"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="412">
   <si>
     <t>STR_key</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -1534,6 +1534,22 @@
   </si>
   <si>
     <t>currentPvESectionCanNotBeSweepedYet</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>此邮件未包含奖励信息</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>thisMailNotContainsRewards</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>此邮件的奖励已经领取</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>theRewardsAlreadyGetedFromThisMail</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1672,7 +1688,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1766">
+  <cellStyleXfs count="1774">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -3443,6 +3459,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3456,7 +3480,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1766">
+  <cellStyles count="1774">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -4342,6 +4366,10 @@
     <cellStyle name="超链接" xfId="1760" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="1762" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="1764" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1766" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1768" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1770" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="1772" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -5220,6 +5248,10 @@
     <cellStyle name="访问过的超链接" xfId="1761" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="1763" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="1765" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1767" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1769" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1771" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="1773" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -5669,10 +5701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="B205" sqref="B205"/>
+      <selection activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -7925,6 +7957,28 @@
         <v>406</v>
       </c>
     </row>
+    <row r="205" spans="1:3" ht="20" customHeight="1">
+      <c r="A205" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B205" s="1">
+        <v>703</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="20" customHeight="1">
+      <c r="A206" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B206" s="1">
+        <v>704</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>